<commit_message>
Foto do Aluno adicionado
</commit_message>
<xml_diff>
--- a/Modelagens/Modelo-Físico-carometro.xlsx
+++ b/Modelagens/Modelo-Físico-carometro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48395996888.INFOSCS\Documents\Batata\Projeto_Carometro\Banco de Dados\Modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D2A338-A690-450A-99A8-2F412520ACF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8F8E51-5067-4ADB-9B85-BD5CA4D76646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{5A179BD2-6D4D-4D8D-B3C3-5F26E31B0FBB}"/>
   </bookViews>
@@ -304,13 +304,13 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -639,10 +639,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -695,13 +695,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -809,10 +809,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -886,12 +886,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -962,7 +962,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,18 +980,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1115,8 +1115,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I7" s="8"/>
+    </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G11" s="10"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>